<commit_message>
add more configuration options;
</commit_message>
<xml_diff>
--- a/ExampleProject/testdata.xlsx
+++ b/ExampleProject/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\funct\Documents\visual studio 2015\Projects\HelperLibrary.Excel\ExampleProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\funct\Source\Repos\HelperLibrary.Excel\ExampleProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -464,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A2:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -476,100 +476,76 @@
     <col min="5" max="5" width="16.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="2">
+      <c r="F2" s="3"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2">
-        <v>23</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C5" s="2">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2">
-        <v>23</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>3</v>
+      </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2">
         <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>3</v>
@@ -578,16 +554,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
         <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>3</v>
@@ -595,34 +571,26 @@
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="2">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C9" s="2">
         <v>23</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="E9" s="4" t="s">
         <v>3</v>
       </c>
@@ -630,16 +598,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C10" s="2">
         <v>23</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>3</v>
@@ -648,34 +616,86 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="2">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A13" s="2">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2">
+        <v>23</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A14" s="2">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2">
-        <v>23</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C14" s="2">
+        <v>23</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="2"/>
+      <c r="E14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E6" r:id="rId4"/>
-    <hyperlink ref="E7" r:id="rId5"/>
-    <hyperlink ref="E9" r:id="rId6"/>
-    <hyperlink ref="E8" r:id="rId7"/>
-    <hyperlink ref="E11" r:id="rId8"/>
-    <hyperlink ref="E10" r:id="rId9"/>
+    <hyperlink ref="E5" r:id="rId1"/>
+    <hyperlink ref="E6" r:id="rId2"/>
+    <hyperlink ref="E7" r:id="rId3"/>
+    <hyperlink ref="E9" r:id="rId4"/>
+    <hyperlink ref="E10" r:id="rId5"/>
+    <hyperlink ref="E12" r:id="rId6"/>
+    <hyperlink ref="E11" r:id="rId7"/>
+    <hyperlink ref="E14" r:id="rId8"/>
+    <hyperlink ref="E13" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>

</xml_diff>